<commit_message>
added to show list overview of all days with number of patients
</commit_message>
<xml_diff>
--- a/records/medical.xlsx
+++ b/records/medical.xlsx
@@ -3,11 +3,12 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="current" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="2024-05-22" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2024-05-23" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -426,10 +427,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -471,12 +472,45 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>segodnja vrach</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
added styles using jinja and base.html
</commit_message>
<xml_diff>
--- a/records/medical.xlsx
+++ b/records/medical.xlsx
@@ -9,6 +9,7 @@
     <sheet name="current" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="2024-05-22" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="2024-05-23" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="2024-05-24" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -427,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:C3"/>
@@ -484,6 +485,21 @@
         </is>
       </c>
       <c r="C3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Vrachhhh</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -526,4 +542,22 @@
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added show specific day patients list, added patients scroll list
</commit_message>
<xml_diff>
--- a/records/medical.xlsx
+++ b/records/medical.xlsx
@@ -1,37 +1,111 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LotusApp\records\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E36E386-5A45-428A-937F-F0B4E657BFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="current" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="2024-05-22" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="2024-05-23" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="2024-05-24" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="current" sheetId="1" r:id="rId1"/>
+    <sheet name="2024-05-22" sheetId="2" r:id="rId2"/>
+    <sheet name="2024-05-23" sheetId="3" r:id="rId3"/>
+    <sheet name="2024-05-24" sheetId="4" r:id="rId4"/>
+    <sheet name="2024-05-25" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="21">
+  <si>
+    <t>дата</t>
+  </si>
+  <si>
+    <t>ФИО врача</t>
+  </si>
+  <si>
+    <t>Всего принято</t>
+  </si>
+  <si>
+    <t>2024-05-22</t>
+  </si>
+  <si>
+    <t>M.V.Vrach</t>
+  </si>
+  <si>
+    <t>2024-05-23</t>
+  </si>
+  <si>
+    <t>segodnja vrach</t>
+  </si>
+  <si>
+    <t>2024-05-24</t>
+  </si>
+  <si>
+    <t>Vrachhhh</t>
+  </si>
+  <si>
+    <t>2024-05-25</t>
+  </si>
+  <si>
+    <t>Arirang</t>
+  </si>
+  <si>
+    <t>Время</t>
+  </si>
+  <si>
+    <t>ФИО пациента</t>
+  </si>
+  <si>
+    <t>Форма</t>
+  </si>
+  <si>
+    <t>ц45647</t>
+  </si>
+  <si>
+    <t>45ц67</t>
+  </si>
+  <si>
+    <t>34ц5657</t>
+  </si>
+  <si>
+    <t>ОАЖЩШОВЭЛТИВ</t>
+  </si>
+  <si>
+    <t>ШАОРЖЩШВОПЭЗ</t>
+  </si>
+  <si>
+    <t>ОЛАВЖЩО</t>
+  </si>
+  <si>
+    <t>ОРАВЖЩШП</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="129"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -50,80 +124,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -423,83 +438,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col width="10.08984375" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="17.81640625" customWidth="1" min="2" max="2"/>
-    <col width="13.1796875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>дата</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>ФИО врача</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Всего принято</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2024-05-22</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>M.V.Vrach</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2024-05-23</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>segodnja vrach</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
         <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2024-05-24</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Vrachhhh</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
         <v>0</v>
       </c>
     </row>
@@ -509,55 +513,309 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3456</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>3456</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>3456</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>3456</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>3456</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>3456</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added input patient field conditionally hidden if not today, added scroll bar on last record)
</commit_message>
<xml_diff>
--- a/records/medical.xlsx
+++ b/records/medical.xlsx
@@ -13,6 +13,7 @@
     <sheet name="2024-05-24" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="2024-05-25" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="2024-05-26" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="2024-05-27" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -444,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
@@ -568,6 +569,26 @@
       <c r="D6" t="inlineStr">
         <is>
           <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Florentiy_Pavlov</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -1202,7 +1223,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45438.8424495309</v>
+        <v>45438.84244952547</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1212,6 +1233,252 @@
       <c r="C5" t="inlineStr">
         <is>
           <t>Р</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Время</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>ФИО пациента</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>М\Ж\Р</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45439.75094185185</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>jbnkjno</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45439.83571817129</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sjfn'pdfi</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45439.83577740741</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>fkmj'fdpk</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45439.83584238426</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>fkmj'fdpk</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>45439.83796740741</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>gdxjchvbk</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45439.83801888889</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>fxckgvbhjk</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45439.83807405092</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>sjfn'pdfi</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45439.83813391204</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>gvkjhkj</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45439.83820114583</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>fkmj'fdpk</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>45439.83825736111</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>jhblk</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>45439.8383075</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>aedf</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>45439.83836677083</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>aedf</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>45439.84088684028</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>fkmj'fdpk</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>45439.85151035563</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>sjfn'pdfi</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>M</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added unique patient name check. added error msg if not unique
</commit_message>
<xml_diff>
--- a/records/medical.xlsx
+++ b/records/medical.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="896" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="896" firstSheet="0" activeTab="10" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="current" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="2024-05-27" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="2024-05-28" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="2024-05-29" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="2024-05-30" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -24,10 +25,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <charset val="129"/>
@@ -42,6 +44,13 @@
       <family val="2"/>
       <color rgb="FF2A2A2A"/>
       <sz val="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="129"/>
+      <family val="2"/>
+      <sz val="8"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -64,12 +73,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -447,10 +457,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -709,6 +719,35 @@
       </c>
       <c r="G9" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-05-30</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Desya_Osipov</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>12</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>6</v>
+      </c>
+      <c r="G10" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -754,6 +793,482 @@
       <c r="E1" t="inlineStr">
         <is>
           <t>Причина</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Время</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ФИО пациента</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>М\Ж\Р</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Дата рождения</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Причина</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Давление</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>45442.46492440972</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>sjfn'pdfi</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>porrkthso[rhk</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>435678</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>45442.4652275</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>gvkjhkj</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>klnm;ksfmg;dfl</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>456879</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>45442.46554097223</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>fkmj'fdpk</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2024-05-07</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>opzdkth</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>456879</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>45442.47230525463</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>gvkjhkj</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>dkjghsropjk</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>456879</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>45442.47873506945</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>gvkjhkj</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2024-05-06</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>fyckuj</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>456879</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>45442.48583460648</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>aedf</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>klnm;ksfmg;dfl</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>456879</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>45442.62278614583</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>gvkjhkj</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2024-05-06</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>klnm;ksfmg;dfl</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>456879</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>45442.62348376158</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>gvkjhkj</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2024-05-06</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>porrkthso[rhk</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>456879</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>45442.62475891204</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>gvkjhkj</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>opzdkth</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>456879</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>45442.63255564815</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>fkmj'fdpk</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>fyckuj</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>435678</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>45442.67932614584</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>jhblk</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2024-01-18</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>tjknlsgk</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>435678</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>45442.7008093287</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>gvkjhkj</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2024-10-08</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>porrkthso[rhk</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>435678</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added logger and exception handler
</commit_message>
<xml_diff>
--- a/records/medical.xlsx
+++ b/records/medical.xlsx
@@ -17,6 +17,7 @@
     <sheet name="2024-05-28" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="2024-05-29" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="2024-05-30" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="2024-05-31" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -457,7 +458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
@@ -748,6 +749,26 @@
       </c>
       <c r="G10" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Karp_Kuzmin</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -1269,6 +1290,57 @@
       <c r="G13" t="inlineStr">
         <is>
           <t>435678</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Время</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>ФИО пациента</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>М\Ж\Р</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Дата рождения</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Причина</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Давление</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
changing indernal folder path to external, bug fixing
</commit_message>
<xml_diff>
--- a/records/medical.xlsx
+++ b/records/medical.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="972" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="972" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="current" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="settings" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="2024-06-01" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="2024-06-02" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -17,9 +18,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,13 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -442,10 +441,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -498,7 +497,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Karp_Kuzmin</t>
+          <t>Karp_Kuzminnn</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -517,6 +516,26 @@
       </c>
       <c r="G2" t="n">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-06-02</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Klara_Novikova</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -648,7 +667,7 @@
   </sheetPr>
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -802,7 +821,7 @@
           <t>4</t>
         </is>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="2" t="n">
         <v>45444.67396430556</v>
       </c>
       <c r="C5" t="inlineStr">
@@ -837,7 +856,7 @@
           <t>5</t>
         </is>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="2" t="n">
         <v>45444.67418059028</v>
       </c>
       <c r="C6" t="inlineStr">
@@ -872,7 +891,7 @@
           <t>6</t>
         </is>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="2" t="n">
         <v>45444.68076171296</v>
       </c>
       <c r="C7" t="inlineStr">
@@ -907,8 +926,8 @@
           <t>7</t>
         </is>
       </c>
-      <c r="B8" s="3" t="n">
-        <v>45444.72288207024</v>
+      <c r="B8" s="2" t="n">
+        <v>45444.72288207176</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -933,6 +952,62 @@
       <c r="G8" t="inlineStr">
         <is>
           <t>456879</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Время</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ФИО пациента</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>М\Ж\Р</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Дата рождения</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Причина</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Давление</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
bug fixing, from unique name+bday removed bday
</commit_message>
<xml_diff>
--- a/records/medical.xlsx
+++ b/records/medical.xlsx
@@ -18,8 +18,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,12 +59,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -444,7 +446,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -497,7 +499,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Karp_Kuzminnn</t>
+          <t>Karp_Kuzmin_records</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -530,12 +532,21 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-1</v>
+        <v>13</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>4</t>
         </is>
+      </c>
+      <c r="E3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -966,13 +977,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -1008,6 +1019,461 @@
       <c r="G1" t="inlineStr">
         <is>
           <t>Давление</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>45445.70815164352</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>sjfn'pdfi</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2006-03-16</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>opzdkth</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>456879</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>45445.70842616898</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>sjfn'pdfi</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2006-03-16</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>fyckuj</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>435678</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>45445.71101790509</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>aedf</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2006-05-18</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>tjknlsgk</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>435678</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>45445.7128197338</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>aedf</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2006-06-01</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>opzdkth</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>456879</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>45445.71299002314</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>gvkjhkj</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2024-05-09</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>tjknlsgk</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>456879</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>45445.79209467593</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>jhk</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>fyckuj</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>435678</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>45445.79244556713</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>sjfn'pdfi</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>opzdkth</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>456879</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>45445.79642175926</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>aedf</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2006-05-29</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>porrkthso[rhk</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>456879</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>45445.81492644676</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>sjfn'pdfi</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2006-05-29</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>dkjghsropjk</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>456879</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>45445.85901008102</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>jhk</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2006-05-30</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>dkjghsropjk</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>456879</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>45445.86378913194</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>jhk</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2006-05-30</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>porrkthso[rhk</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>435678</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>45445.8720893287</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>jhk</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2006-05-30</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>tjknlsgk</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>456879</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="n">
+        <v>45445.87463234954</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>jhkgfguhjk</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2006-05-29</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>dkjghsropjk</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>435678</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
modified business logic. each patient will have different doctor
</commit_message>
<xml_diff>
--- a/records/medical.xlsx
+++ b/records/medical.xlsx
@@ -3,13 +3,15 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="972" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="972" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="current" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="settings" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="2024-06-01" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="2024-06-02" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="2024-07-09" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="2024-07-10" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -18,9 +20,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -59,13 +60,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -443,17 +443,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
     <col width="10.08984375" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="17.81640625" customWidth="1" min="2" max="2"/>
-    <col width="13.1796875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="13.1796875" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -462,30 +461,20 @@
           <t>дата</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>ФИО врача</t>
-        </is>
-      </c>
-      <c r="C1" t="n">
+      <c r="B1" t="n">
         <v>0</v>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>id_doctor</t>
+          <t>Ж</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
-        <is>
-          <t>Р</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Ж</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
         <is>
           <t>М</t>
         </is>
@@ -497,26 +486,16 @@
           <t>2024-06-01</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Karp_Kuzmin_records</t>
-        </is>
+      <c r="B2" t="n">
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="n">
         <v>3</v>
       </c>
     </row>
@@ -526,27 +505,55 @@
           <t>2024-06-02</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Klara_Novikova</t>
-        </is>
+      <c r="B3" t="n">
+        <v>12</v>
       </c>
       <c r="C3" t="n">
-        <v>13</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6</v>
       </c>
       <c r="E3" t="n">
         <v>3</v>
       </c>
-      <c r="F3" t="n">
-        <v>7</v>
-      </c>
-      <c r="G3" t="n">
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-07-10</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -977,7 +984,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1343,8 +1350,8 @@
           <t>10</t>
         </is>
       </c>
-      <c r="B11" s="3" t="n">
-        <v>45445.85901008102</v>
+      <c r="B11" s="2" t="n">
+        <v>45445.86062358796</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1358,17 +1365,17 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2006-05-30</t>
+          <t>2006-05-29</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>dkjghsropjk</t>
+          <t>porrkthso[rhk</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>456879</t>
+          <t>435678</t>
         </is>
       </c>
     </row>
@@ -1378,8 +1385,8 @@
           <t>11</t>
         </is>
       </c>
-      <c r="B12" s="3" t="n">
-        <v>45445.86378913194</v>
+      <c r="B12" s="2" t="n">
+        <v>45445.860871875</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1393,17 +1400,17 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2006-05-30</t>
+          <t>2006-05-29</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>porrkthso[rhk</t>
+          <t>dkjghsropjk</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>435678</t>
+          <t>456879</t>
         </is>
       </c>
     </row>
@@ -1413,12 +1420,12 @@
           <t>12</t>
         </is>
       </c>
-      <c r="B13" s="3" t="n">
-        <v>45445.8720893287</v>
+      <c r="B13" s="2" t="n">
+        <v>45445.87829535879</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>jhk</t>
+          <t>jhkjhblijho</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1428,12 +1435,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2006-05-30</t>
+          <t>2006-05-29</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>tjknlsgk</t>
+          <t>fyckuj</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1442,38 +1449,306 @@
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="B14" s="3" t="n">
-        <v>45445.87463234954</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>jhkgfguhjk</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <cols>
+    <col width="17.81640625" bestFit="1" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Время</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ФИО пациента</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>М\Ж\Р</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Дата рождения</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Причина</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Давление</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Врач</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Врач_Индекс</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>45482.79670672453</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>шортшотш</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>Ж</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>2006-05-29</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>dkjghsropjk</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>435678</t>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2006-04-06</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>рототщто</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>7890</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <cols>
+    <col width="17.81640625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="11.7265625" bestFit="1" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Время</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ФИО пациента</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Врач</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Врач_Индекс</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>М\Ж\Р</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Дата рождения</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Причина</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Давление</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>45483.5933899537</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ааонег</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Karp_Kuzmin</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2006-07-04</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>шкгпщш</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>7890</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>45483.59384497685</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>квгнгпрщщж</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Karp_Kuzmin</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2006-07-03</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>dstfui</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>ytfu67589</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>45483.59436456019</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>рпплродж</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Karp_Kuzmin</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2006-07-03</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>utfuygu</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>678</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added fill form and save to folder
</commit_message>
<xml_diff>
--- a/records/medical.xlsx
+++ b/records/medical.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="972" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="current" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="settings" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="2024-06-01" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="2024-06-02" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="2024-07-09" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="2024-07-10" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="current" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="settings" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-06-01" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-06-02" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-07-09" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-07-10" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-07-12" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -20,8 +21,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -60,12 +62,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -443,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -553,6 +556,25 @@
         <v>1</v>
       </c>
       <c r="E5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-07-12</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1755,4 +1777,285 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Время</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ФИО пациента</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Врач</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Врач_Индекс</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>М\Ж\Р</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Дата рождения</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Причина</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Давление</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>45485.24525712963</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>iurhosthk</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Karp_Kuzmin</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2006-07-04</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>рототщто</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>7890</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>45485.25785924769</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>dxdjkughi</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Karp_Kuzmin</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>jgfghol</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>4689</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>45485.81736980324</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>jykugk</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Karp_Kuzmin</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2006-07-03</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>dstfui</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>7890</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>45485.83415211806</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>patient name</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Yefrem_Lebedev</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2006-07-03</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>reason beseda</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>pressure</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>45485.83810637737</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>patient test</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Desya_Osipov</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2006-07-11</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>beseda osipov</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>pressure test</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated fill form. started filtering patients data table
</commit_message>
<xml_diff>
--- a/records/medical.xlsx
+++ b/records/medical.xlsx
@@ -13,6 +13,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-07-09" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-07-10" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-07-12" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-07-13" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -446,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -576,6 +577,25 @@
       </c>
       <c r="E6" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-07-13</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2019,7 +2039,7 @@
         </is>
       </c>
       <c r="B6" s="3" t="n">
-        <v>45485.83810637737</v>
+        <v>45485.83810637731</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -2052,6 +2072,287 @@
       <c r="I6" t="inlineStr">
         <is>
           <t>pressure test</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Время</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ФИО пациента</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Врач</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Врач_Индекс</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>М\Ж\Р</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Дата рождения</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Причина</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Давление</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>45486.68052039352</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>patient test</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Karp_Kuzmin</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2006-07-03</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>рототщто</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>54678908</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>45486.68202555556</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>opatient name</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Yefrem_Lebedev</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2006-07-10</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>utfuygu</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>54678908</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>45486.83163686343</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>patient test name</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Karp_Kuzmin</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2006-07-03</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>reason</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>678</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>45486.83648765046</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Irina Vorontsova Klementjevna</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Karp_Kuzmin</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Ж</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2002-01-08</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>obshee obsledowanie</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>7890</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>45486.83918565972</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Kiril Vodjanow Viktorovitch</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Yefrem_Lebedev</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>jalobi na kashel</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>678</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added filter to show table rows by selected doctor:
</commit_message>
<xml_diff>
--- a/records/medical.xlsx
+++ b/records/medical.xlsx
@@ -14,6 +14,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-07-10" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-07-12" sheetId="7" state="visible" r:id="rId7"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-07-13" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-07-14" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -447,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -596,6 +597,16 @@
       </c>
       <c r="E7" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-07-14</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -2359,4 +2370,70 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Время</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ФИО пациента</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Врач</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Врач_Индекс</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>М\Ж\Р</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Дата рождения</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Причина</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Давление</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
first corrections after test. Added more specific info for error msg.
</commit_message>
<xml_diff>
--- a/records/medical.xlsx
+++ b/records/medical.xlsx
@@ -9,6 +9,7 @@
     <sheet name="current" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="settings" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="2024-07-25" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="2024-09-21" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -440,7 +441,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -494,6 +495,16 @@
       </c>
       <c r="E2" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -1163,4 +1174,70 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Время</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ФИО пациента</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Врач</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Врач_Индекс</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>М\Ж\Р</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Дата рождения</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Причина</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Давление</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
corrected doctor status and saving
</commit_message>
<xml_diff>
--- a/records/medical.xlsx
+++ b/records/medical.xlsx
@@ -1231,7 +1231,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>on</t>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>on</t>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1301,7 +1301,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>n/a</t>
+          <t>n/ahjk</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1331,7 +1331,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>on</t>
+          <t>false</t>
         </is>
       </c>
     </row>

</xml_diff>